<commit_message>
chnages to cems id's
</commit_message>
<xml_diff>
--- a/public/data/CMMS.xlsx
+++ b/public/data/CMMS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1808,30 +1808,30 @@
   </sheetPr>
   <dimension ref="A1:Q233"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A193" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B219" activeCellId="0" sqref="B219"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.9234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="64.3928571428571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="224.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="64.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="27.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="224.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13379,7 +13379,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>